<commit_message>
added lodash, implemented recursion because while loop did not work out correctly, rewrote some functions
</commit_message>
<xml_diff>
--- a/excel/1995/Report-1995-01-11.xlsx
+++ b/excel/1995/Report-1995-01-11.xlsx
@@ -11,39 +11,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="183">
-  <si>
-    <t>recall_classification_date</t>
-  </si>
-  <si>
-    <t>product_type</t>
-  </si>
-  <si>
-    <t>classification</t>
-  </si>
-  <si>
-    <t>recall_number</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>recalling_firm</t>
-  </si>
-  <si>
-    <t>manufacturer</t>
-  </si>
-  <si>
-    <t>recall_initiation_date</t>
-  </si>
-  <si>
-    <t>reason</t>
-  </si>
-  <si>
-    <t>volume</t>
-  </si>
-  <si>
-    <t>distribution</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="184">
+  <si>
+    <t>RECALL_CLASSIFICATION_DATE</t>
+  </si>
+  <si>
+    <t>PRODUCT_TYPE</t>
+  </si>
+  <si>
+    <t>CLASSIFICATION</t>
+  </si>
+  <si>
+    <t>RECALL_NUMBER</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>RECALLING_FIRM</t>
+  </si>
+  <si>
+    <t>MANUFACTURER</t>
+  </si>
+  <si>
+    <t>RECALL_INITIALIZATION_DATE</t>
+  </si>
+  <si>
+    <t>REASON</t>
+  </si>
+  <si>
+    <t>VOLUME</t>
+  </si>
+  <si>
+    <t>DISTRIBUTION</t>
   </si>
   <si>
     <t>1995-01-11</t>
@@ -52,376 +52,376 @@
     <t>Drugs</t>
   </si>
   <si>
-    <t xml:space="preserve"> II=</t>
+    <t>II</t>
   </si>
   <si>
     <t>d-042-5</t>
   </si>
   <si>
-    <t>cleocin Phosphate 600 Mg/50 Ml Iv Solution, An Antibiotic</t>
-  </si>
-  <si>
-    <t>the Upjohn Company</t>
-  </si>
-  <si>
-    <t>baxter Healthcare Corporation, Carolina, puerto Rico</t>
-  </si>
-  <si>
-    <t>January 10, 1994</t>
-  </si>
-  <si>
-    <t>some Product Carton Covers Incorrectly Declare The Strength as 900 Mg/50 Ml Instead Of 600 Mg/50 Ml</t>
-  </si>
-  <si>
-    <t>13,032 bags were distributed; firm estimates none remains on the market</t>
-  </si>
-  <si>
-    <t>nationwide</t>
+    <t>Cleocin Phosphate 600 Mg 50 Ml Iv Solution An Antibiotic</t>
+  </si>
+  <si>
+    <t>The Upjohn Company</t>
+  </si>
+  <si>
+    <t>Baxter Healthcare Corporation Carolina Puerto Rico</t>
+  </si>
+  <si>
+    <t>January 10 1994</t>
+  </si>
+  <si>
+    <t>Some Product Carton Covers Incorrectly Declare The Strength As 900 Mg 50 Ml Instead Of 600 Mg 50 Ml</t>
+  </si>
+  <si>
+    <t>13 032 Bags Were Distributed Firm Estimates None Remains On The Market</t>
+  </si>
+  <si>
+    <t>Nationwide</t>
   </si>
   <si>
     <t>d-043-5</t>
   </si>
   <si>
-    <t>touro La Caplet, In 100 Caplet Bottles, Rx Drug Indicated  as A Time Released Decongestant/expectorant</t>
-  </si>
-  <si>
-    <t>dartmouth Pharmaceuticals</t>
-  </si>
-  <si>
-    <t>wildflower Pharmacal Corporation, Mineola, New York</t>
-  </si>
-  <si>
-    <t>December 28, 1994</t>
-  </si>
-  <si>
-    <t>product Does Not Meet Time Release Specifications</t>
-  </si>
-  <si>
-    <t>3,839 100-caplet bottles and 34,500 unit dose caplets were distributed</t>
-  </si>
-  <si>
-    <t>massachusetts, Maine, Connecticut, Georgia, New York, New Jersey</t>
+    <t>Touro La Caplet In 100 Caplet Bottles Rx Drug Indicated As A Time Released Decongestant Expectorant</t>
+  </si>
+  <si>
+    <t>Dartmouth Pharmaceuticals</t>
+  </si>
+  <si>
+    <t>Wildflower Pharmacal Corporation Mineola New York</t>
+  </si>
+  <si>
+    <t>December 28 1994</t>
+  </si>
+  <si>
+    <t>Product Does Not Meet Time Release Specifications</t>
+  </si>
+  <si>
+    <t>3 839 100 Caplet Bottles And 34 500 Unit Dose Caplets Were Distributed</t>
+  </si>
+  <si>
+    <t>Massachusetts Maine Connecticut Georgia New York New Jersey</t>
   </si>
   <si>
     <t>Biologics</t>
   </si>
   <si>
-    <t xml:space="preserve"> I==</t>
+    <t>I</t>
   </si>
   <si>
     <t>b-125-5</t>
   </si>
   <si>
-    <t>pk "r" Syringe, Catalog #2m1361</t>
-  </si>
-  <si>
-    <t>olympus American</t>
-  </si>
-  <si>
-    <t>olympus Optical Company, Ltd</t>
-  </si>
-  <si>
-    <t>September 28, 1994</t>
-  </si>
-  <si>
-    <t>olympus Brand 2 Pk7100 Instrument Syringes, Packed In Boxes  that Were Mislabeled As Containing Larger Syringes, Were  distributed</t>
-  </si>
-  <si>
-    <t>24 units</t>
-  </si>
-  <si>
-    <t>Oklahoma, Missouri, North Carolina, Pennsylvania, Michigan, Massachusetts, Wisconsin, Texas, Arizona, New Jersey, Washington State, Rhode Island, California, New York, Canada</t>
+    <t>Pk R Syringe Catalog 2 M 1361</t>
+  </si>
+  <si>
+    <t>Olympus American</t>
+  </si>
+  <si>
+    <t>Olympus Optical Company Ltd</t>
+  </si>
+  <si>
+    <t>September 28 1994</t>
+  </si>
+  <si>
+    <t>Olympus Brand 2 Pk 7100 Instrument Syringes Packed In Boxes That Were Mislabeled As Containing Larger Syringes Were Distributed</t>
+  </si>
+  <si>
+    <t>24 Units</t>
+  </si>
+  <si>
+    <t>Oklahoma Missouri North Carolina Pennsylvania Michigan Massachusetts Wisconsin Texas Arizona New Jersey Washington State Rhode Island California New York Canada</t>
   </si>
   <si>
     <t>b-126/132-5</t>
   </si>
   <si>
-    <t>(a) Whole Blood; (b) Red Blood Cells; (c) Red Blood Cells, for Further Manufacture; (d) Platelets; (e) Platelets, expired; (f) Fresh Frozen Plasma; (g) Recovered Plasma</t>
-  </si>
-  <si>
-    <t>blood Systems</t>
-  </si>
-  <si>
-    <t>blood Systems, Inc</t>
-  </si>
-  <si>
-    <t>April 28, 1994</t>
-  </si>
-  <si>
-    <t>blood Products, Collected In A Manner That Compromises The sterility Of The Collection System, Were Distributed</t>
-  </si>
-  <si>
-    <t>(a) 9 units; (b) 1,888 units; (c) 6 units; (d) 1,253 units;
-(e) 4 units; (f) 862 units; (g) 32 units</t>
-  </si>
-  <si>
-    <t>nationwide And International</t>
+    <t>A Whole Blood B Red Blood Cells C Red Blood Cells For Further Manufacture D Platelets E Platelets Expired F Fresh Frozen Plasma G Recovered Plasma</t>
+  </si>
+  <si>
+    <t>Blood Systems</t>
+  </si>
+  <si>
+    <t>Blood Systems Inc</t>
+  </si>
+  <si>
+    <t>April 28 1994</t>
+  </si>
+  <si>
+    <t>Blood Products Collected In A Manner That Compromises The Sterility Of The Collection System Were Distributed</t>
+  </si>
+  <si>
+    <t>A 9 Units B 1 888 Units C 6 Units D 1 253 Units E 4 Units F 862 Units G 32 Units</t>
+  </si>
+  <si>
+    <t>Nationwide And International</t>
   </si>
   <si>
     <t>b-135-5</t>
   </si>
   <si>
-    <t>red Blood Cells</t>
-  </si>
-  <si>
-    <t>american National Red Cross (the), Columbus, Ohio</t>
-  </si>
-  <si>
-    <t>July 8, 1994</t>
-  </si>
-  <si>
-    <t>blood Product, Which Was Collected From A Donor Who Admitted  to Visiting An Area Designated As Endemic For Malaria, Was  distributed</t>
-  </si>
-  <si>
-    <t>1 unit</t>
-  </si>
-  <si>
-    <t>ohio</t>
+    <t>Red Blood Cells</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>American National Red Cross The Columbus Ohio</t>
+  </si>
+  <si>
+    <t>July 8 1994</t>
+  </si>
+  <si>
+    <t>Blood Product Which Was Collected From A Donor Who Admitted To Visiting An Area Designated As Endemic For Malaria Was Distributed</t>
+  </si>
+  <si>
+    <t>1 Unit</t>
+  </si>
+  <si>
+    <t>Ohio</t>
   </si>
   <si>
     <t>b-137-5</t>
   </si>
   <si>
-    <t>the American National Red Cross, Charlotte, North Carolina</t>
-  </si>
-  <si>
-    <t>June 7, 1994</t>
-  </si>
-  <si>
-    <t>blood Products, Collected From An Ineligible Donor Due To A  reported History Of Cancer, Were Distributed</t>
-  </si>
-  <si>
-    <t>2 unit</t>
-  </si>
-  <si>
-    <t>north Carolina, Tennessee</t>
+    <t>The American National Red Cross Charlotte North Carolina</t>
+  </si>
+  <si>
+    <t>June 7 1994</t>
+  </si>
+  <si>
+    <t>Blood Products Collected From An Ineligible Donor Due To A Reported History Of Cancer Were Distributed</t>
+  </si>
+  <si>
+    <t>2 Unit</t>
+  </si>
+  <si>
+    <t>North Carolina Tennessee</t>
   </si>
   <si>
     <t>b-141/142-5</t>
   </si>
   <si>
-    <t>(a) Red Blood Cells, Frozen; (b) Platelets, Pheresis</t>
+    <t>A Red Blood Cells Frozen B Platelets Pheresis</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>the American National Red Cross, Miami, Florida, By  telephone October 8, 1993, Followed By Letter October 20, 1993</t>
-  </si>
-  <si>
-    <t>unknown recall date</t>
-  </si>
-  <si>
-    <t>blood Products, Incorrectly Tested For Syphilis, Were distributed</t>
-  </si>
-  <si>
-    <t>1 unit of each component</t>
-  </si>
-  <si>
-    <t>florida</t>
+    <t>The American National Red Cross Miami Florida By Telephone October 8 1993 Followed By Letter October 20 1993</t>
+  </si>
+  <si>
+    <t>N A</t>
+  </si>
+  <si>
+    <t>Blood Products Incorrectly Tested For Syphilis Were Distributed</t>
+  </si>
+  <si>
+    <t>1 Unit Of Each Component</t>
+  </si>
+  <si>
+    <t>Florida</t>
   </si>
   <si>
     <t>b-147-5</t>
   </si>
   <si>
-    <t>Midland County Hospital District, Doing  business As Permian Basin Regional Blood Center</t>
-  </si>
-  <si>
-    <t>July 29, 1993</t>
-  </si>
-  <si>
-    <t>blood Product, Collected From A Therapeutic Donor And Not labeled To Indicate The Type Of Donor And Disease State, Was Distributed</t>
-  </si>
-  <si>
-    <t>texas</t>
+    <t>Midland County Hospital District Doing Business As Permian Basin Regional Blood Center</t>
+  </si>
+  <si>
+    <t>July 29 1993</t>
+  </si>
+  <si>
+    <t>Blood Product Collected From A Therapeutic Donor And Not Labeled To Indicate The Type Of Donor And Disease State Was Distributed</t>
+  </si>
+  <si>
+    <t>Texas</t>
   </si>
   <si>
     <t>b-149-5</t>
   </si>
   <si>
-    <t>source Plasma</t>
-  </si>
-  <si>
-    <t>community Bio Resources</t>
-  </si>
-  <si>
-    <t>immuno-u</t>
-  </si>
-  <si>
-    <t>June 14, 1994</t>
-  </si>
-  <si>
-    <t>blood Product, Which Tested Non-reactive For Hepatitis B  surface Antigen (hbsag), But Was Collected From A Donor Who  previously Tested Repeatedly Reactive For Hbsag, Was  distributed</t>
-  </si>
-  <si>
-    <t>austria</t>
+    <t>Source Plasma</t>
+  </si>
+  <si>
+    <t>Community Bio Resources</t>
+  </si>
+  <si>
+    <t>Immuno U</t>
+  </si>
+  <si>
+    <t>June 14 1994</t>
+  </si>
+  <si>
+    <t>Blood Product Which Tested Non Reactive For Hepatitis B Surface Antigen Hbsag But Was Collected From A Donor Who Previously Tested Repeatedly Reactive For Hbsag Was Distributed</t>
+  </si>
+  <si>
+    <t>Austria</t>
   </si>
   <si>
     <t>b-150-5</t>
   </si>
   <si>
-    <t>community Bio Resources, Inc</t>
-  </si>
-  <si>
-    <t>blood Products, Which Tested Non-reactive For Hepatitis B surface Antigen (hbsag), But Were Collected From A Donor Who Previously Tested Repeatedly Reactive For Hbsag, Were distributed</t>
-  </si>
-  <si>
-    <t>116 units</t>
-  </si>
-  <si>
-    <t>michigan, New Jersey, Austria</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> III</t>
+    <t>Community Bio Resources Inc</t>
+  </si>
+  <si>
+    <t>Blood Products Which Tested Non Reactive For Hepatitis B Surface Antigen Hbsag But Were Collected From A Donor Who Previously Tested Repeatedly Reactive For Hbsag Were Distributed</t>
+  </si>
+  <si>
+    <t>116 Units</t>
+  </si>
+  <si>
+    <t>Michigan New Jersey Austria</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
   <si>
     <t>b-136-5</t>
   </si>
   <si>
-    <t>recovered Plasma</t>
-  </si>
-  <si>
-    <t>the American National Red Cross, Boise, Idaho</t>
-  </si>
-  <si>
-    <t>December 1, 1993</t>
-  </si>
-  <si>
-    <t>blood Product, Corresponding To A Unit Of Red Blood Cells found To Be Contaminated With Serratia Liquefaciens Was distributed</t>
-  </si>
-  <si>
-    <t>california</t>
+    <t>Recovered Plasma</t>
+  </si>
+  <si>
+    <t>The American National Red Cross Boise Idaho</t>
+  </si>
+  <si>
+    <t>December 1 1993</t>
+  </si>
+  <si>
+    <t>Blood Product Corresponding To A Unit Of Red Blood Cells Found To Be Contaminated With Serratia Liquefaciens Was Distributed</t>
+  </si>
+  <si>
+    <t>California</t>
   </si>
   <si>
     <t>b-138-5</t>
   </si>
   <si>
-    <t>June 24, 1994</t>
-  </si>
-  <si>
-    <t>blood Product, Collected From An Ineligible Donor Due To A reported History Of Cancer, Was Distributed</t>
-  </si>
-  <si>
-    <t>2 units</t>
+    <t>June 24 1994</t>
+  </si>
+  <si>
+    <t>Blood Product Collected From An Ineligible Donor Due To A Reported History Of Cancer Was Distributed</t>
+  </si>
+  <si>
+    <t>2 Units</t>
   </si>
   <si>
     <t>b-139/140-5</t>
   </si>
   <si>
-    <t>(a) Platelets, Pheresis; (b) Leukocytes</t>
-  </si>
-  <si>
-    <t>July 19, 1994</t>
-  </si>
-  <si>
-    <t>blood Products, That Were Either Incorrectly Tested For antibodies To Human Immunodeficiency Virus Types 1 And 2  (anti-hiv-1/2; Or Incorrectly Tested For Anti-hiv-1/2 And  antibody To Hepatitis B Core Antigen (anti-hbc), Were distributed</t>
-  </si>
-  <si>
-    <t>(a) 33 units; (b) 6 units</t>
-  </si>
-  <si>
-    <t>(a) Georgia, North Carolina; (b) North Carolina</t>
+    <t>A Platelets Pheresis B Leukocytes</t>
+  </si>
+  <si>
+    <t>July 19 1994</t>
+  </si>
+  <si>
+    <t>Blood Products That Were Either Incorrectly Tested For Antibodies To Human Immunodeficiency Virus Types 1 And 2 Anti Hiv 1 2 Or Incorrectly Tested For Anti Hiv 1 2 And Antibody To Hepatitis B Core Antigen Anti Hbc Were Distributed</t>
+  </si>
+  <si>
+    <t>A 33 Units B 6 Units</t>
+  </si>
+  <si>
+    <t>A Georgia North Carolina B North Carolina</t>
   </si>
   <si>
     <t>b-143-5</t>
   </si>
   <si>
-    <t>platelets</t>
-  </si>
-  <si>
-    <t>houchin Community Blood Bank, Bakersfield, California</t>
-  </si>
-  <si>
-    <t>September 22, 1994</t>
-  </si>
-  <si>
-    <t>blood Products, Which Were Exposed To Unacceptable Storage Temperatures, Were Distributed</t>
-  </si>
-  <si>
-    <t>17 units</t>
+    <t>Platelets</t>
+  </si>
+  <si>
+    <t>Houchin Community Blood Bank Bakersfield California</t>
+  </si>
+  <si>
+    <t>September 22 1994</t>
+  </si>
+  <si>
+    <t>Blood Products Which Were Exposed To Unacceptable Storage Temperatures Were Distributed</t>
+  </si>
+  <si>
+    <t>17 Units</t>
   </si>
   <si>
     <t>b-144-5</t>
   </si>
   <si>
-    <t>plasma</t>
-  </si>
-  <si>
-    <t>united Blood Services Blood Systems, Inc</t>
-  </si>
-  <si>
-    <t>July 7, 1994</t>
-  </si>
-  <si>
-    <t>plasma, Prepared Later Than Eight Hours After Phlebotomy And Mislabeled As Fresh Frozen Plasma, Was Distributed</t>
+    <t>Plasma</t>
+  </si>
+  <si>
+    <t>United Blood Services Blood Systems Inc</t>
+  </si>
+  <si>
+    <t>July 7 1994</t>
+  </si>
+  <si>
+    <t>Plasma Prepared Later Than Eight Hours After Phlebotomy And Mislabeled As Fresh Frozen Plasma Was Distributed</t>
   </si>
   <si>
     <t>b-145-5</t>
   </si>
   <si>
-    <t>midland County Hospital District, Doing Business As Permian  basin Regional Blood Center, Midland, Texas</t>
-  </si>
-  <si>
-    <t>October 14, 1993</t>
-  </si>
-  <si>
-    <t>autologous Blood Product, That Tested Repeatedly Reactive  for Hepatitis B Surface Antigen (hbsag) But Was Not appropriately Labeled To Reflect The Hbsag Reactive Result, was Distributed</t>
+    <t>Midland County Hospital District Doing Business As Permian Basin Regional Blood Center Midland Texas</t>
+  </si>
+  <si>
+    <t>October 14 1993</t>
+  </si>
+  <si>
+    <t>Autologous Blood Product That Tested Repeatedly Reactive For Hepatitis B Surface Antigen Hbsag But Was Not Appropriately Labeled To Reflect The Hbsag Reactive Result Was Distributed</t>
   </si>
   <si>
     <t>b-146-5</t>
   </si>
   <si>
-    <t>corzyme Hepatitis B Core Antigen (recombinant Diagnostic kit</t>
-  </si>
-  <si>
-    <t>abbott Laboratories, Abbott Park, Illinois</t>
-  </si>
-  <si>
-    <t>October 19, 1994</t>
-  </si>
-  <si>
-    <t>antibody To Hepatitis B Core Antigen (anti-hbc) Test Kits, that May Demonstrate Increased Reactive Rates, Were Distributed</t>
-  </si>
-  <si>
-    <t>538 test kits were distributed; firm estimates none remains
-on the market</t>
-  </si>
-  <si>
-    <t>nationwide And Canada</t>
+    <t>Corzyme Hepatitis B Core Antigen Recombinant Diagnostic Kit</t>
+  </si>
+  <si>
+    <t>Abbott Laboratories Abbott Park Illinois</t>
+  </si>
+  <si>
+    <t>October 19 1994</t>
+  </si>
+  <si>
+    <t>Antibody To Hepatitis B Core Antigen Anti Hbc Test Kits That May Demonstrate Increased Reactive Rates Were Distributed</t>
+  </si>
+  <si>
+    <t>538 Test Kits Were Distributed Firm Estimates None Remains On The Market</t>
+  </si>
+  <si>
+    <t>Nationwide And Canada</t>
   </si>
   <si>
     <t>b-148-5</t>
   </si>
   <si>
-    <t>inland Northwest Blood Center, Spokane, Washington</t>
-  </si>
-  <si>
-    <t>January 27, 1994</t>
-  </si>
-  <si>
-    <t>blood Products Labeled With Incorrect Expiration Dates Were Distributed</t>
-  </si>
-  <si>
-    <t>4 units</t>
-  </si>
-  <si>
-    <t>washington State</t>
+    <t>Inland Northwest Blood Center Spokane Washington</t>
+  </si>
+  <si>
+    <t>January 27 1994</t>
+  </si>
+  <si>
+    <t>Blood Products Labeled With Incorrect Expiration Dates Were Distributed</t>
+  </si>
+  <si>
+    <t>4 Units</t>
+  </si>
+  <si>
+    <t>Washington State</t>
   </si>
   <si>
     <t>b-151-5</t>
   </si>
   <si>
-    <t>hivab Antibodies To Human Immunodeficiency Virus Types 1 And 2 Test Kits</t>
-  </si>
-  <si>
-    <t>November 30, 1994</t>
-  </si>
-  <si>
-    <t>antibody To Human Immunodeficiency Virus Types 1 And 2 (anti-hiv-1/2) Test Kits, That May Demonstrate Increased  reactive Rates, Were Distributed</t>
-  </si>
-  <si>
-    <t>6,100 kits were distributed; firm estimated that 1,500 kits
-remained on market at time of recall initiation</t>
+    <t>Hivab Antibodies To Human Immunodeficiency Virus Types 1 And 2 Test Kits</t>
+  </si>
+  <si>
+    <t>November 30 1994</t>
+  </si>
+  <si>
+    <t>Antibody To Human Immunodeficiency Virus Types 1 And 2 Anti Hiv 1 2 Test Kits That May Demonstrate Increased Reactive Rates Were Distributed</t>
+  </si>
+  <si>
+    <t>6 100 Kits Were Distributed Firm Estimated That 1 500 Kits Remained On Market At Time Of Recall Initiation</t>
   </si>
   <si>
     <t>Devices</t>
@@ -430,142 +430,139 @@
     <t>z-205/207-5</t>
   </si>
   <si>
-    <t>ophthalmic Surgical Devices: (a) Storz Premiere 24hr</t>
-  </si>
-  <si>
-    <t>storz Instrument Company, St</t>
-  </si>
-  <si>
-    <t>May 6, 1994</t>
-  </si>
-  <si>
-    <t>pinhole Leaks Were Found In The Tyvek Plastic Side Of The  pouches Used To Package The Products, Which Could Cause The sterility To Be Compromised</t>
-  </si>
-  <si>
-    <t>(a) 8,085 units were distributed between 7/31/91 and 
-3/30/94; (b) 637 units were distributed between 7/31/91 and
-3/24/94; (c) 1,289 units were distributed between 7/31/94 
-and 4/8/94</t>
+    <t>Ophthalmic Surgical Devices A Storz Premiere 24 Hr</t>
+  </si>
+  <si>
+    <t>Storz Instrument Company St</t>
+  </si>
+  <si>
+    <t>May 6 1994</t>
+  </si>
+  <si>
+    <t>Pinhole Leaks Were Found In The Tyvek Plastic Side Of The Pouches Used To Package The Products Which Could Cause The Sterility To Be Compromised</t>
+  </si>
+  <si>
+    <t>A 8 085 Units Were Distributed Between 7 31 91 And 3 30 94 B 637 Units Were Distributed Between 7 31 91 And 3 24 94 C 1 289 Units Were Distributed Between 7 31 94 And 4 8 94</t>
   </si>
   <si>
     <t>z-230/232-5</t>
   </si>
   <si>
-    <t>upsizing Sleeves, Models 033-240, 030-221, And 033-210 When  used In The Ventricular Channel Of The Reflex 8223e Pulse generator</t>
-  </si>
-  <si>
-    <t>telectronics Pacing Systems</t>
-  </si>
-  <si>
-    <t>telectronics Pacing Systems, Miami Lakes, Florida</t>
-  </si>
-  <si>
-    <t>September 30, 1994</t>
-  </si>
-  <si>
-    <t>the Leads Used With The Above Models Of Upsizing Sleeves May not Allow For A Proper Connection In The Ventricular Channel of The Reflex 8223e Pulse Generator</t>
-  </si>
-  <si>
-    <t>1,691 units were distributed</t>
+    <t>Upsizing Sleeves Models 033 240 030 221 And 033 210 When Used In The Ventricular Channel Of The Reflex 8223 E Pulse Generator</t>
+  </si>
+  <si>
+    <t>Telectronics Pacing Systems</t>
+  </si>
+  <si>
+    <t>Telectronics Pacing Systems Miami Lakes Florida</t>
+  </si>
+  <si>
+    <t>September 30 1994</t>
+  </si>
+  <si>
+    <t>The Leads Used With The Above Models Of Upsizing Sleeves May Not Allow For A Proper Connection In The Ventricular Channel Of The Reflex 8223 E Pulse Generator</t>
+  </si>
+  <si>
+    <t>1 691 Units Were Distributed</t>
   </si>
   <si>
     <t>z-238/240-5</t>
   </si>
   <si>
-    <t>pacesetter "afp" Multi-mode/programmable Cardiac Pulse generators (pacemaker Or Pacer): (a) Model 275; (b)  model 281; (c) Model 283</t>
-  </si>
-  <si>
-    <t>pacesetter</t>
-  </si>
-  <si>
-    <t>pacesetter, Inc</t>
-  </si>
-  <si>
-    <t>October 17, 1994</t>
-  </si>
-  <si>
-    <t>a Defective Crystal In The "afp" Pacer, Causes The Device To suddenly Stop Operating</t>
-  </si>
-  <si>
-    <t>181 units</t>
+    <t>Pacesetter Afp Multi Mode Programmable Cardiac Pulse Generators Pacemaker Or Pacer A Model 275 B Model 281 C Model 283</t>
+  </si>
+  <si>
+    <t>Pacesetter</t>
+  </si>
+  <si>
+    <t>Pacesetter Inc</t>
+  </si>
+  <si>
+    <t>October 17 1994</t>
+  </si>
+  <si>
+    <t>A Defective Crystal In The Afp Pacer Causes The Device To Suddenly Stop Operating</t>
+  </si>
+  <si>
+    <t>181 Units</t>
   </si>
   <si>
     <t>z-241-5</t>
   </si>
   <si>
-    <t>wizard Personal Organizer And Pacemaker Database, Software revision 1</t>
-  </si>
-  <si>
-    <t>telectronics Pacing Systems, Englewood, Colorado</t>
-  </si>
-  <si>
-    <t>August 1, 1994</t>
-  </si>
-  <si>
-    <t>the Firm Failed To File A 510(k) Pre-market Notification For  their Wizard Personal Organizer, Software Revision 1  database</t>
-  </si>
-  <si>
-    <t>218 total version 1 cards were distributed</t>
+    <t>Wizard Personal Organizer And Pacemaker Database Software Revision 1</t>
+  </si>
+  <si>
+    <t>Telectronics Pacing Systems Englewood Colorado</t>
+  </si>
+  <si>
+    <t>August 1 1994</t>
+  </si>
+  <si>
+    <t>The Firm Failed To File A 510 K Pre Market Notification For Their Wizard Personal Organizer Software Revision 1 Database</t>
+  </si>
+  <si>
+    <t>218 Total Version 1 Cards Were Distributed</t>
   </si>
   <si>
     <t>z-246/251-5</t>
   </si>
   <si>
-    <t>cordis Webster Braided-tip Deflectable Electrophysiology  catheters, Indicated For Electrophysiological Mapping Of cardiac Structures: (a) Model D78; (b) Model D88;  (c) Model D7-270; (d) Model 1104; (e) Model 1105;  (f) Model 1108</t>
-  </si>
-  <si>
-    <t>cordis Webster, Inc</t>
-  </si>
-  <si>
-    <t>October 26, 1994</t>
-  </si>
-  <si>
-    <t>the Tip Electrode Can Come Loose Due To Lack Of Bond  adhesion Caused By The Dacron Braid Material Interacting  With The Polyurethane Adhesive</t>
-  </si>
-  <si>
-    <t>approximately 5,390 units were distributed</t>
+    <t>Cordis Webster Braided Tip Deflectable Electrophysiology Catheters Indicated For Electrophysiological Mapping Of Cardiac Structures A Model D 78 B Model D 88 C Model D 7 270 D Model 1104 E Model 1105 F Model 1108</t>
+  </si>
+  <si>
+    <t>Cordis Webster Inc</t>
+  </si>
+  <si>
+    <t>October 26 1994</t>
+  </si>
+  <si>
+    <t>The Tip Electrode Can Come Loose Due To Lack Of Bond Adhesion Caused By The Dacron Braid Material Interacting With The Polyurethane Adhesive</t>
+  </si>
+  <si>
+    <t>Approximately 5 390 Units Were Distributed</t>
   </si>
   <si>
     <t>z-202/204-5</t>
   </si>
   <si>
-    <t>first Choice Blood Glucose Test Strips For The Glucometer 3  Meter: (a) Catalog #91060, Bottle Of 50 Strips;  (b) Catalog #91061, Two Bottles Of 50 Strips; (c) Catalog #91065, Blister Pack Of 50 Strips</t>
-  </si>
-  <si>
-    <t>polymer Technology International (pti) Issaquah, Washington</t>
-  </si>
-  <si>
-    <t>September 6, 1994</t>
-  </si>
-  <si>
-    <t>the Blood Glucose Strips Could Provide Low Patient Results</t>
-  </si>
-  <si>
-    <t>61,119 bottles were distributed</t>
-  </si>
-  <si>
-    <t>nationwide, Argentina, Lebanon, Pakistan</t>
+    <t>First Choice Blood Glucose Test Strips For The Glucometer 3 Meter A Catalog 91060 Bottle Of 50 Strips B Catalog 91061 Two Bottles Of 50 Strips C Catalog 91065 Blister Pack Of 50 Strips</t>
+  </si>
+  <si>
+    <t>Polymer Technology International Pti Issaquah Washington</t>
+  </si>
+  <si>
+    <t>September 6 1994</t>
+  </si>
+  <si>
+    <t>The Blood Glucose Strips Could Provide Low Patient Results</t>
+  </si>
+  <si>
+    <t>61 119 Bottles Were Distributed</t>
+  </si>
+  <si>
+    <t>Nationwide Argentina Lebanon Pakistan</t>
   </si>
   <si>
     <t>z-218-5</t>
   </si>
   <si>
-    <t>difco Bacto Blood Collectors, Product #1832-30, Intended For Collecting Blood Samples Used In Clinical Diagnosis</t>
-  </si>
-  <si>
-    <t>difco Laboratories</t>
-  </si>
-  <si>
-    <t>deltar - Diamed Operation, Elk Grove Village, illinois</t>
-  </si>
-  <si>
-    <t>October 11, 1994</t>
-  </si>
-  <si>
-    <t>the 21 Gauge Winged Venipuncture Needle May Be Covered With a Hard Brown Rust-like Coating</t>
-  </si>
-  <si>
-    <t>67,000 units were distributed</t>
+    <t>Difco Bacto Blood Collectors Product 1832 30 Intended For Collecting Blood Samples Used In Clinical Diagnosis</t>
+  </si>
+  <si>
+    <t>Difco Laboratories</t>
+  </si>
+  <si>
+    <t>Deltar Diamed Operation Elk Grove Village Illinois</t>
+  </si>
+  <si>
+    <t>October 11 1994</t>
+  </si>
+  <si>
+    <t>The 21 Gauge Winged Venipuncture Needle May Be Covered With A Hard Brown Rust Like Coating</t>
+  </si>
+  <si>
+    <t>67 000 Units Were Distributed</t>
   </si>
 </sst>
 </file>
@@ -1137,22 +1134,22 @@
         <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1166,28 +1163,28 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
         <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1201,28 +1198,28 @@
         <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1236,28 +1233,28 @@
         <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
         <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1271,28 +1268,28 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1306,28 +1303,28 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1338,31 +1335,31 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H12" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I12" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1373,31 +1370,31 @@
         <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" t="s">
+        <v>95</v>
+      </c>
+      <c r="I13" t="s">
+        <v>96</v>
+      </c>
+      <c r="J13" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" t="s">
         <v>93</v>
-      </c>
-      <c r="E13" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" t="s">
-        <v>94</v>
-      </c>
-      <c r="I13" t="s">
-        <v>95</v>
-      </c>
-      <c r="J13" t="s">
-        <v>96</v>
-      </c>
-      <c r="K13" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1408,31 +1405,31 @@
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="I14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K14" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1443,31 +1440,31 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H15" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I15" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J15" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="K15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1478,31 +1475,31 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F16" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1513,31 +1510,31 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E17" t="s">
         <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H17" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I17" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1548,31 +1545,31 @@
         <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F18" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G18" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I18" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J18" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K18" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1583,31 +1580,31 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E19" t="s">
         <v>49</v>
       </c>
       <c r="F19" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I19" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J19" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K19" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1618,28 +1615,28 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E20" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F20" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="I20" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K20" t="s">
         <v>47</v>
@@ -1650,31 +1647,31 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F21" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G21" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H21" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I21" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K21" t="s">
         <v>47</v>
@@ -1685,31 +1682,31 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
         <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E22" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F22" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G22" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H22" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I22" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J22" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K22" t="s">
         <v>47</v>
@@ -1720,31 +1717,31 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E23" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F23" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G23" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H23" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I23" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J23" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K23" t="s">
         <v>47</v>
@@ -1755,31 +1752,31 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
         <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E24" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F24" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H24" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J24" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K24" t="s">
         <v>47</v>
@@ -1790,31 +1787,31 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E25" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F25" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H25" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J25" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K25" t="s">
         <v>47</v>
@@ -1825,34 +1822,34 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D26" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E26" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F26" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="G26" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H26" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I26" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J26" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K26" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1860,31 +1857,31 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E27" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F27" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G27" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H27" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I27" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="J27" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="K27" t="s">
         <v>47</v>

</xml_diff>